<commit_message>
updated the datafiles and the pre analysis script to make it reproducible
</commit_message>
<xml_diff>
--- a/1_data/data_irn_food_controls.xlsx
+++ b/1_data/data_irn_food_controls.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3992432-04E6-4142-9389-F6BEE9BDA561}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F38F61E-5B6A-445E-AE45-7788F2A26680}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -470,7 +470,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,6 +766,9 @@
       <c r="D14">
         <v>6278.8</v>
       </c>
+      <c r="E14">
+        <v>5733.2</v>
+      </c>
       <c r="F14" t="s">
         <v>36</v>
       </c>
@@ -783,6 +786,9 @@
       <c r="D15">
         <v>6238.6</v>
       </c>
+      <c r="E15">
+        <v>5745</v>
+      </c>
       <c r="F15" t="s">
         <v>36</v>
       </c>
@@ -799,6 +805,9 @@
       </c>
       <c r="D16">
         <v>6120.9</v>
+      </c>
+      <c r="E16">
+        <v>5695.1</v>
       </c>
       <c r="F16" t="s">
         <v>36</v>

</xml_diff>